<commit_message>
#22 | Config json file to convert weather data
</commit_message>
<xml_diff>
--- a/Mapping.xlsx
+++ b/Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INTERN\BingNewsTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB2030E-1B8D-4225-B867-554D70375C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E61AD88-2EC1-4ADB-A8B5-D56B80094251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{2956BAC4-AC4A-4147-9DDC-AADB6F4F41FF}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
   <si>
     <t>title</t>
   </si>
@@ -183,13 +183,49 @@
   </si>
   <si>
     <t>config</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>◢</t>
+  </si>
+  <si>
+    <t>ns + obj.SouPropertyPath</t>
+  </si>
+  <si>
+    <t>{{https://trends.google.com/trends/trendingsearches/daily}picture}</t>
+  </si>
+  <si>
+    <t>System.Xml.Linq.XName</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>current.condition.icon</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>current.humidity</t>
+  </si>
+  <si>
+    <t>current.feelslike_c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -201,6 +237,21 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -227,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -235,27 +286,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -271,7 +382,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -567,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D256996-630A-4D62-B202-A77F7FC87DFD}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -795,17 +906,50 @@
         <v>34</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="6"/>
+    </row>
   </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="1">
+    <mergeCell ref="C26:C34"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD731C0-E516-44BA-86A9-80AC5E855560}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -817,7 +961,7 @@
     <col min="5" max="5" width="17.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -828,7 +972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -839,7 +983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -853,7 +997,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -867,7 +1011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -878,7 +1022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -889,7 +1033,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -900,12 +1044,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -916,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -927,7 +1071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -938,7 +1082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -947,6 +1091,33 @@
       </c>
       <c r="C13" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="7"/>
+      <c r="E16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -960,52 +1131,52 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.19921875" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="6" max="6" width="19.69921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.8984375" customWidth="1"/>
     <col min="8" max="8" width="12.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1019,7 +1190,7 @@
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F3" t="s">
@@ -1036,7 +1207,7 @@
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="6"/>
       <c r="F4" t="s">
         <v>46</v>
       </c>
@@ -1045,49 +1216,73 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E5" s="4"/>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
       <c r="L5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E6" s="4"/>
+      <c r="E6" s="6"/>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E7" s="4"/>
+      <c r="E7" s="6"/>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E8" s="4"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E9" s="4"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E10" s="4"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E11" s="4"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E12" s="4"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E13" s="4"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E14" s="4"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E15" s="4"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E16" s="4"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17" s="4"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E18" s="4"/>
+      <c r="E18" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
#53 | Create controller bingnews &  test service
</commit_message>
<xml_diff>
--- a/Mapping.xlsx
+++ b/Mapping.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INTERN\BingNewsTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E61AD88-2EC1-4ADB-A8B5-D56B80094251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA16D53-CDC1-413C-8E2E-ACFC82615270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{2956BAC4-AC4A-4147-9DDC-AADB6F4F41FF}"/>
+    <workbookView xWindow="3432" yWindow="1704" windowWidth="17280" windowHeight="9420" activeTab="3" xr2:uid="{2956BAC4-AC4A-4147-9DDC-AADB6F4F41FF}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
     <sheet name="RSS" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="API_Controller" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
   <si>
     <t>title</t>
   </si>
@@ -219,17 +220,41 @@
   </si>
   <si>
     <t>current.feelslike_c</t>
+  </si>
+  <si>
+    <t>Trending  new panel</t>
+  </si>
+  <si>
+    <t>List&lt;Article&gt;</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>IconChannel</t>
+  </si>
+  <si>
+    <t>LikeNumber</t>
+  </si>
+  <si>
+    <t>DisLikeNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -238,7 +263,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -246,14 +271,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -338,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -346,12 +379,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -363,6 +390,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -379,6 +416,129 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Ngoặc móc Trái 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{638973E1-6B9B-4B6F-5B45-B895296360F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2560320" y="167640"/>
+          <a:ext cx="373380" cy="1089660"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="vi-VN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Mũi tên: Xuống 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F1C871F-2354-23AD-A97E-E0D4017CF87A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2286000" y="220980"/>
+          <a:ext cx="76200" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="vi-VN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -684,14 +844,14 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="27.796875" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -702,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -713,7 +873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -724,7 +884,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -735,7 +895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -746,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -757,7 +917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -768,7 +928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -779,13 +939,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -796,7 +956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -807,7 +967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -818,7 +978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -829,7 +989,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -840,7 +1000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -851,7 +1011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -862,7 +1022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -873,7 +1033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -884,7 +1044,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -895,7 +1055,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
@@ -906,34 +1066,34 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C26" s="6" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="6"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="6"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="9"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -952,16 +1112,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" customWidth="1"/>
-    <col min="4" max="4" width="13.296875" customWidth="1"/>
-    <col min="5" max="5" width="17.8984375" customWidth="1"/>
+    <col min="1" max="1" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -972,7 +1132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -983,7 +1143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -997,7 +1157,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1011,7 +1171,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1022,7 +1182,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1033,7 +1193,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1044,12 +1204,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1060,7 +1220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1071,7 +1231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1082,7 +1242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1093,30 +1253,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="7"/>
-      <c r="E16" s="8" t="s">
+    <row r="15" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="5"/>
+      <c r="E16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="4:7" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="9" t="s">
+    <row r="17" spans="4:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="8" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1130,34 +1290,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04505A68-7F98-48F1-A717-2E4CA7026BBC}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.19921875" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="6" max="6" width="19.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.8984375" customWidth="1"/>
-    <col min="8" max="8" width="12.3984375" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
@@ -1180,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1190,7 +1350,7 @@
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="9" t="s">
         <v>50</v>
       </c>
       <c r="F3" t="s">
@@ -1200,14 +1360,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="9"/>
       <c r="F4" t="s">
         <v>46</v>
       </c>
@@ -1215,14 +1375,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="9"/>
       <c r="F5" t="s">
         <v>60</v>
       </c>
@@ -1233,8 +1393,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E6" s="6"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E6" s="9"/>
       <c r="F6" t="s">
         <v>62</v>
       </c>
@@ -1242,8 +1402,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E7" s="6"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E7" s="9"/>
       <c r="F7" t="s">
         <v>63</v>
       </c>
@@ -1251,38 +1411,38 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E18" s="6"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1292,4 +1452,78 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D6A01E-5255-450F-ABE5-4FD615AE50DC}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#70 | Handle sample interaction data, created user table. Write trigger, fuction, and constraint for sql
</commit_message>
<xml_diff>
--- a/Mapping.xlsx
+++ b/Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INTERN\BingNewsTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA16D53-CDC1-413C-8E2E-ACFC82615270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B79FF61-33AA-4237-BCC4-9271AF94C7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3432" yWindow="1704" windowWidth="17280" windowHeight="9420" activeTab="3" xr2:uid="{2956BAC4-AC4A-4147-9DDC-AADB6F4F41FF}"/>
+    <workbookView xWindow="3108" yWindow="1440" windowWidth="17280" windowHeight="9420" activeTab="3" xr2:uid="{2956BAC4-AC4A-4147-9DDC-AADB6F4F41FF}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
   <si>
     <t>title</t>
   </si>
@@ -244,6 +244,24 @@
   </si>
   <si>
     <t>DisLikeNumber</t>
+  </si>
+  <si>
+    <t>UserInteraction</t>
+  </si>
+  <si>
+    <t>IdUser</t>
+  </si>
+  <si>
+    <t>Guid</t>
+  </si>
+  <si>
+    <t>IdArticle</t>
+  </si>
+  <si>
+    <t>Like</t>
+  </si>
+  <si>
+    <t>DisLike</t>
   </si>
 </sst>
 </file>
@@ -391,15 +409,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1067,33 +1085,33 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="11" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="9"/>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="9"/>
+      <c r="C28" s="11"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="9"/>
+      <c r="C29" s="11"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="9"/>
+      <c r="C30" s="11"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C31" s="9"/>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C32" s="9"/>
+      <c r="C32" s="11"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="9"/>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="9"/>
+      <c r="C34" s="11"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1304,18 +1322,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1350,7 +1368,7 @@
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F3" t="s">
@@ -1367,7 +1385,7 @@
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="11"/>
       <c r="F4" t="s">
         <v>46</v>
       </c>
@@ -1382,7 +1400,7 @@
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="11"/>
       <c r="F5" t="s">
         <v>60</v>
       </c>
@@ -1394,7 +1412,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E6" s="9"/>
+      <c r="E6" s="11"/>
       <c r="F6" t="s">
         <v>62</v>
       </c>
@@ -1403,7 +1421,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="9"/>
+      <c r="E7" s="11"/>
       <c r="F7" t="s">
         <v>63</v>
       </c>
@@ -1412,37 +1430,37 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="9"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="9"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="9"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="9"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="9"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="9"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="9"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="9"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E16" s="9"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="9"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="9"/>
+      <c r="E18" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1456,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D6A01E-5255-450F-ABE5-4FD615AE50DC}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,61 +1485,91 @@
     <col min="1" max="1" width="22.7265625" customWidth="1"/>
     <col min="2" max="2" width="12.453125" customWidth="1"/>
     <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="F1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
       <c r="C2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
       <c r="C3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="12" t="s">
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
       <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
       <c r="C6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
       <c r="C7" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:A7"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
#72 | Handle Parallel in C#
</commit_message>
<xml_diff>
--- a/Mapping.xlsx
+++ b/Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INTERN\BingNewsTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B79FF61-33AA-4237-BCC4-9271AF94C7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCC8B4E-B9BB-4F96-B188-FDEC6399DFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3108" yWindow="1440" windowWidth="17280" windowHeight="9420" activeTab="3" xr2:uid="{2956BAC4-AC4A-4147-9DDC-AADB6F4F41FF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{2956BAC4-AC4A-4147-9DDC-AADB6F4F41FF}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
   <si>
     <t>title</t>
   </si>
@@ -262,6 +262,17 @@
   </si>
   <si>
     <t>DisLike</t>
+  </si>
+  <si>
+    <t>UserClickEvent</t>
+  </si>
+  <si>
+    <t>1. Gộp nhóm lại có ArticleId cùng channel, cùng 
+category,
+2. Đếm và sắp xếp giảm dần theo channel, cate
+3. chọn ra các bản tin tương tự khoảng 50% trong top 10
+theo phần trăm tổng 60%
+40% còn lại  xử lý trùng các kênh đã đăng ký</t>
   </si>
 </sst>
 </file>
@@ -389,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -418,6 +429,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1474,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D6A01E-5255-450F-ABE5-4FD615AE50DC}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I5" sqref="I5:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,9 +1503,10 @@
     <col min="2" max="2" width="12.453125" customWidth="1"/>
     <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.08984375" customWidth="1"/>
+    <col min="10" max="10" width="33.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>64</v>
       </c>
@@ -1502,8 +1520,12 @@
         <v>72</v>
       </c>
       <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="C2" t="s">
         <v>68</v>
@@ -1514,8 +1536,14 @@
       <c r="G2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="C3" t="s">
         <v>69</v>
@@ -1526,8 +1554,14 @@
       <c r="G3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="10" t="s">
         <v>66</v>
@@ -1542,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="C5" t="s">
         <v>13</v>
@@ -1553,23 +1587,41 @@
       <c r="G5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="C6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="C7" t="s">
         <v>71</v>
       </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:A7"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I5:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>